<commit_message>
Updated to correct some bugs
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt\Dropbox\Heartland\Scripts\NR-Importer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Dropbox\Heartland\Scripts\NR-Importer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Config" sheetId="4" r:id="rId2"/>
     <sheet name="OriginalData" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Network Summary</t>
   </si>
@@ -146,12 +146,15 @@
   </si>
   <si>
     <t>CLOSET1-VL10</t>
+  </si>
+  <si>
+    <t>Option43</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -483,29 +486,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.5546875" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" customWidth="1"/>
-    <col min="15" max="16" width="17.109375" customWidth="1"/>
-    <col min="17" max="17" width="25.5546875" customWidth="1"/>
-    <col min="18" max="18" width="14.88671875" customWidth="1"/>
-    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" customWidth="1"/>
+    <col min="15" max="17" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="25.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.85546875" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -552,34 +555,37 @@
         <v>11</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -639,39 +645,43 @@
         <v>24h</v>
       </c>
       <c r="P2" t="str">
-        <f>Config!B$10</f>
+        <f>Config!B$10 &amp; ""</f>
+        <v/>
+      </c>
+      <c r="Q2" t="str">
+        <f>Config!B$11 &amp; ""</f>
         <v>2.2.2.2</v>
       </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
         <f>Config!B$3</f>
         <v>30m</v>
       </c>
-      <c r="R2" t="str">
+      <c r="S2" t="str">
         <f>Config!B$4</f>
         <v>1m</v>
       </c>
-      <c r="S2" t="str">
+      <c r="T2" t="str">
         <f>Config!B$5</f>
         <v>1.1.1.1,1.1.1.2</v>
       </c>
-      <c r="T2" t="str">
+      <c r="U2" t="str">
         <f>Config!B$6</f>
         <v>1.1.1.1</v>
       </c>
-      <c r="U2" t="str">
+      <c r="V2" t="str">
         <f>Config!B$7</f>
         <v>1.1.1.2</v>
-      </c>
-      <c r="V2">
-        <f>Config!B$9</f>
-        <v>0</v>
       </c>
       <c r="W2">
         <f>Config!B$9</f>
         <v>0</v>
       </c>
-      <c r="X2" t="str">
-        <f>Config!B$10</f>
+      <c r="X2">
+        <f>Config!B$9</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" t="str">
+        <f>Config!B$11</f>
         <v>2.2.2.2</v>
       </c>
     </row>
@@ -685,16 +695,16 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -702,7 +712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -710,7 +720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -718,7 +728,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -726,7 +736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -734,7 +744,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -742,7 +752,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -750,7 +760,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -758,7 +768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -766,15 +776,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -784,7 +799,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -794,7 +809,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
@@ -804,7 +819,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -814,7 +829,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -824,7 +839,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -834,7 +849,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -844,7 +859,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -854,7 +869,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -864,7 +879,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -887,14 +902,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -926,7 +941,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -964,9 +979,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1128,26 +1146,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9BB02E6-050F-4A70-87F0-6E8E7E45CA43}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14B7622E-F157-4219-ADE7-8DD88067D3F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="e8104dc4-b7a5-4754-9af3-5e67fd30ee26"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1171,9 +1178,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14B7622E-F157-4219-ADE7-8DD88067D3F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9BB02E6-050F-4A70-87F0-6E8E7E45CA43}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="e8104dc4-b7a5-4754-9af3-5e67fd30ee26"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>